<commit_message>
SE AGREGO FECHA DE INGRESO DUAL
</commit_message>
<xml_diff>
--- a/SisDualultimo/web/doc/cat_alumnos.xlsx
+++ b/SisDualultimo/web/doc/cat_alumnos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovani\Desktop\catalogo de dual\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gioca\Desktop\pruebas DUAL\ALUMNOS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C75644-7F1B-4682-A61F-31D69D1ECCDB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E523384-C803-4F5F-A275-1E6222D8E505}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17244" windowHeight="5580" xr2:uid="{438593B8-E1F0-476D-B82F-ED4480F61AB8}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{438593B8-E1F0-476D-B82F-ED4480F61AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>MATRICULA</t>
   </si>
@@ -79,12 +79,18 @@
   </si>
   <si>
     <t>CLAVE_CARRERA</t>
+  </si>
+  <si>
+    <t>FECHA_INGRESO_DUAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -114,8 +120,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -430,10 +437,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DF869E-4E6C-48BE-896A-B95D4A508C07}">
-  <dimension ref="A1:P1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -444,10 +451,11 @@
     <col min="12" max="13" width="22.88671875" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="13.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,6 +503,9 @@
       </c>
       <c r="P1" t="s">
         <v>13</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
tablero completo universidAd COMPLETO
</commit_message>
<xml_diff>
--- a/SisDualultimo/web/doc/cat_alumnos.xlsx
+++ b/SisDualultimo/web/doc/cat_alumnos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gioca\Desktop\pruebas DUAL\ALUMNOS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Giovani\Desktop\catalogo de dual\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4E523384-C803-4F5F-A275-1E6222D8E505}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C75644-7F1B-4682-A61F-31D69D1ECCDB}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{438593B8-E1F0-476D-B82F-ED4480F61AB8}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17244" windowHeight="5580" xr2:uid="{438593B8-E1F0-476D-B82F-ED4480F61AB8}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
   <si>
     <t>MATRICULA</t>
   </si>
@@ -79,18 +79,12 @@
   </si>
   <si>
     <t>CLAVE_CARRERA</t>
-  </si>
-  <si>
-    <t>FECHA_INGRESO_DUAL</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="dd/mm/yyyy;@"/>
-  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -120,9 +114,8 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -437,10 +430,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8DF869E-4E6C-48BE-896A-B95D4A508C07}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:P1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -451,11 +444,10 @@
     <col min="12" max="13" width="22.88671875" customWidth="1"/>
     <col min="14" max="14" width="19" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="21.44140625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.44140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="13.5546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -503,9 +495,6 @@
       </c>
       <c r="P1" t="s">
         <v>13</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>